<commit_message>
Tablas de objetos DMG
</commit_message>
<xml_diff>
--- a/excels/Core/Trad DMG.xlsx
+++ b/excels/Core/Trad DMG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rol\Roll20\Repos github\5etoolsEsp\excels\Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2442AB5-17CC-4134-BFBD-3D4AEEAB081A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39DF356-3A17-428A-8640-D025182289BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="854" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="854" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indice" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="1388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="1399">
   <si>
     <t>quickref</t>
   </si>
@@ -4198,13 +4198,46 @@
   </si>
   <si>
     <t>Granada de humo</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos I</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos H</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos G</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos F</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos E</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos D</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos C</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos B</t>
+  </si>
+  <si>
+    <t>Tabla de Objetos Mágicos A</t>
+  </si>
+  <si>
+    <t>Varita de relámpagos</t>
+  </si>
+  <si>
+    <t>Varita de parálisis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4222,14 +4255,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -4257,7 +4282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4282,7 +4307,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4694,7 +4718,7 @@
   <dimension ref="B1:C202"/>
   <sheetViews>
     <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5274,46 +5298,73 @@
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>1396</v>
+      </c>
       <c r="C112" t="s">
         <v>1271</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>1395</v>
+      </c>
       <c r="C113" t="s">
         <v>1272</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>1394</v>
+      </c>
       <c r="C114" t="s">
         <v>1273</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>1393</v>
+      </c>
       <c r="C115" t="s">
         <v>1274</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>1392</v>
+      </c>
       <c r="C116" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>1391</v>
+      </c>
       <c r="C117" t="s">
         <v>1276</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>1390</v>
+      </c>
       <c r="C118" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>1389</v>
+      </c>
       <c r="C119" t="s">
         <v>1278</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>1388</v>
+      </c>
       <c r="C120" t="s">
         <v>1279</v>
       </c>
@@ -6058,8 +6109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:D512"/>
   <sheetViews>
-    <sheetView topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="C356" sqref="C356"/>
+    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0">
+      <selection activeCell="D469" sqref="D469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6865,7 +6916,7 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="10" t="s">
+      <c r="B100" t="s">
         <v>1068</v>
       </c>
       <c r="C100" t="s">
@@ -10009,6 +10060,9 @@
       </c>
     </row>
     <row r="493" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B493" t="s">
+        <v>1397</v>
+      </c>
       <c r="C493" t="s">
         <v>488</v>
       </c>
@@ -10038,6 +10092,9 @@
       </c>
     </row>
     <row r="497" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B497" t="s">
+        <v>1398</v>
+      </c>
       <c r="C497" t="s">
         <v>491</v>
       </c>
@@ -10177,8 +10234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10387,7 +10444,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>958</v>
       </c>
@@ -10395,7 +10452,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>959</v>
       </c>
@@ -10403,7 +10460,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>847</v>
       </c>
@@ -10411,7 +10468,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>941</v>
       </c>
@@ -10419,7 +10476,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>1069</v>
       </c>
@@ -10427,7 +10484,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>1102</v>
       </c>
@@ -10435,7 +10492,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>966</v>
       </c>
@@ -10443,7 +10500,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>968</v>
       </c>
@@ -10451,7 +10508,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>1085</v>
       </c>
@@ -10459,7 +10516,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>970</v>
       </c>
@@ -10467,7 +10524,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>1115</v>
       </c>
@@ -10475,7 +10532,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>1104</v>
       </c>
@@ -10483,7 +10540,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>797</v>
       </c>
@@ -10491,7 +10548,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>798</v>
       </c>

</xml_diff>